<commit_message>
Add flag for debug and testing
</commit_message>
<xml_diff>
--- a/data/Template_structure.xlsx
+++ b/data/Template_structure.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Objects" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="112">
   <si>
     <t xml:space="preserve">Instanzname</t>
   </si>
@@ -326,16 +326,10 @@
     <t xml:space="preserve">Input Parameter 2</t>
   </si>
   <si>
-    <t xml:space="preserve">IN_Prm_2ö</t>
-  </si>
-  <si>
     <t xml:space="preserve">Input Parameter 3</t>
   </si>
   <si>
     <t xml:space="preserve">Input Parameter 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IN_Prm_4ä</t>
   </si>
   <si>
     <t xml:space="preserve">Input Parameter 5</t>
@@ -491,8 +485,8 @@
   </sheetPr>
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1608,8 +1602,8 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1655,13 +1649,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>99</v>
+        <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>96</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1672,18 +1666,18 @@
         <v>96</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>96</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1734,7 +1728,7 @@
         <v>96</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1745,7 +1739,7 @@
         <v>96</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1756,7 +1750,7 @@
         <v>96</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1767,7 +1761,7 @@
         <v>96</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1778,7 +1772,7 @@
         <v>96</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1827,10 +1821,10 @@
         <v>14</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1876,13 +1870,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1928,13 +1922,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1980,13 +1974,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>113</v>
-      </c>
       <c r="C2" s="0" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished validation check of the data
</commit_message>
<xml_diff>
--- a/data/Template_structure.xlsx
+++ b/data/Template_structure.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="111">
   <si>
     <t xml:space="preserve">Instanzname</t>
   </si>
@@ -357,9 +357,6 @@
   </si>
   <si>
     <t xml:space="preserve">Dummy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bool</t>
   </si>
   <si>
     <t xml:space="preserve">REAL</t>
@@ -486,7 +483,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1603,7 +1600,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1699,7 +1696,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1794,7 +1791,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1846,12 +1843,12 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.86"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
@@ -1873,7 +1870,7 @@
         <v>109</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>109</v>
@@ -1898,7 +1895,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1925,7 +1922,7 @@
         <v>109</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>109</v>
@@ -1950,7 +1947,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1977,7 +1974,7 @@
         <v>109</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>109</v>

</xml_diff>

<commit_message>
clean ups for beta release
</commit_message>
<xml_diff>
--- a/data/Template_structure.xlsx
+++ b/data/Template_structure.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="75">
   <si>
     <t xml:space="preserve">Instanzname</t>
   </si>
@@ -198,114 +198,6 @@
   </si>
   <si>
     <t xml:space="preserve">"DB_FB_Std".Object10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Object11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FB11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"DB_FB_Std".Object11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Object12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FB12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"DB_FB_Std".Object12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Object13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FB13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"DB_FB_Std".Object13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Object14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FB14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"DB_FB_Std".Object14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Object15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FB15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"DB_FB_Std".Object15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Object16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FB16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"DB_FB_Std".Object16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Object17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FB17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"DB_FB_Std".Object17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Object18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FB18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"DB_FB_Std".Object18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Object19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FB19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"DB_FB_Std".Object19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Object20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FB20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"DB_FB_Std".Object20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Object21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FB21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"DB_FB_Std".Object21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Object22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FB22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"DB_FB_Std".Object22</t>
   </si>
   <si>
     <t xml:space="preserve">Name</t>
@@ -480,10 +372,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1015,570 +907,6 @@
       </c>
       <c r="O11" s="0" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I12" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J12" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K12" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="L12" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="M12" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="N12" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="O12" s="0" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I13" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J13" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K13" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="L13" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="M13" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="N13" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="O13" s="0" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="10.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I14" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J14" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K14" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="L14" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="M14" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="N14" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="O14" s="0" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I15" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J15" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K15" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="L15" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="M15" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="N15" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="O15" s="0" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J16" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K16" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="L16" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="M16" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="N16" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="O16" s="0" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="L17" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="M17" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="N17" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="O17" s="0" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K18" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="L18" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="M18" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="N18" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="O18" s="0" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I19" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K19" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="L19" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="M19" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="N19" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="O19" s="0" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I20" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J20" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K20" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="L20" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="M20" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="N20" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="O20" s="0" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H21" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J21" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K21" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="L21" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="M21" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="N21" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="O21" s="0" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J22" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K22" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="L22" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="M22" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="N22" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="O22" s="0" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G23" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J23" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K23" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="L23" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="M23" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="N23" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="O23" s="0" t="s">
-        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1613,13 +941,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1627,10 +955,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>97</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1638,10 +966,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>98</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1649,10 +977,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1660,10 +988,10 @@
         <v>7</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1671,10 +999,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1708,13 +1036,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1722,10 +1050,10 @@
         <v>9</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>102</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1733,10 +1061,10 @@
         <v>10</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>103</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1744,10 +1072,10 @@
         <v>11</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>104</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1755,10 +1083,10 @@
         <v>12</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>105</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1766,10 +1094,10 @@
         <v>13</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1804,13 +1132,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1818,10 +1146,10 @@
         <v>14</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>107</v>
+        <v>71</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>108</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1856,24 +1184,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>109</v>
+        <v>73</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>109</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1908,24 +1236,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>109</v>
+        <v>73</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>109</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1960,24 +1288,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>109</v>
+        <v>73</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>110</v>
+        <v>74</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>109</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>